<commit_message>
Bo sung them giao dien va tinh nang add data
</commit_message>
<xml_diff>
--- a/form_collectdata/form_collect/DataCollected/final_new.xlsx
+++ b/form_collectdata/form_collect/DataCollected/final_new.xlsx
@@ -487,12 +487,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK6"/>
+  <dimension ref="A1:BK19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1257,10 +1257,645 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Phạm Thành Đạt</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>B20DCDT049</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>D20DTMT1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Phạm Hoàng Anh</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Nguyễn Trọng Đức</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>B20DCDT057</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>D20XLTH</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Phạm Hoàng Anh</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Đào Huy Hùng</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>B20DCDT081</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>D20DTMT1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Phạm Hoàng Anh</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Ngô Hải Long</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>B20DCDT119</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>D20DTRB</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Phạm Văn Sự</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Nguyễn Xuân Khoa</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>B20DCDT111</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>D20DTRB</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Phạm Văn Sự</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Nguyễn Trọng Hưởng</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>B20DCDT099</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>D20DTMT2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Phạm Văn Sự</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>5.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Nguyễn Quang Hưng</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>B20DCDT098</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>D20DTMT1</t>
+        </is>
+      </c>
+      <c r="AM13" t="inlineStr">
+        <is>
+          <t>Phạm Văn Sự</t>
+        </is>
+      </c>
+      <c r="AN13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AO13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Giáp Thị Huyền</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>B20DCDT092</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>D20DTMT2</t>
+        </is>
+      </c>
+      <c r="AM14" t="inlineStr">
+        <is>
+          <t>Trần Thị Thúy Hà</t>
+        </is>
+      </c>
+      <c r="AN14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AO14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AP14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Tạ Ngọc Bích</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>B20DCDT020</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>D20DTMT2</t>
+        </is>
+      </c>
+      <c r="AX15" t="inlineStr">
+        <is>
+          <t>Lương Công Duẩn</t>
+        </is>
+      </c>
+      <c r="AY15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AZ15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BB15" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="BC15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Nguyễn Xuân Mai</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>B20DCDT127</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>D20DTMT2</t>
+        </is>
+      </c>
+      <c r="AX16" t="inlineStr">
+        <is>
+          <t>Trần Tuấn Anh</t>
+        </is>
+      </c>
+      <c r="AY16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AZ16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BA16" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="BB16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BC16" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BD16" t="inlineStr">
+        <is>
+          <t>3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>La Thị Hồng Nhung</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>B20DCDT158</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>D20XLTH</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Phạm Hoàng Anh</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>3.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Nguyễn Trung Tuấn</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>B20DCDT190</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>D20XLTH</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Phạm Hoàng Anh</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>3.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Tạ Hồng Hải</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>B20DCDT064</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>D20XLTH</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr"/>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="inlineStr"/>
+      <c r="AK19" t="inlineStr"/>
+      <c r="AL19" t="inlineStr"/>
+      <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr"/>
+      <c r="AO19" t="inlineStr"/>
+      <c r="AP19" t="inlineStr"/>
+      <c r="AQ19" t="inlineStr"/>
+      <c r="AR19" t="inlineStr"/>
+      <c r="AS19" t="inlineStr"/>
+      <c r="AT19" t="inlineStr"/>
+      <c r="AU19" t="inlineStr"/>
+      <c r="AV19" t="inlineStr"/>
+      <c r="AW19" t="inlineStr"/>
+      <c r="AX19" t="inlineStr">
+        <is>
+          <t>Lê Đức Toàn</t>
+        </is>
+      </c>
+      <c r="AY19" t="inlineStr"/>
+      <c r="AZ19" t="inlineStr"/>
+      <c r="BA19" t="inlineStr"/>
+      <c r="BB19" t="inlineStr"/>
+      <c r="BC19" t="inlineStr"/>
+      <c r="BD19" t="inlineStr"/>
+      <c r="BE19" t="inlineStr"/>
+      <c r="BF19" t="inlineStr"/>
+      <c r="BG19" t="inlineStr"/>
+      <c r="BH19" t="inlineStr"/>
+      <c r="BI19" t="inlineStr"/>
+      <c r="BJ19" t="inlineStr"/>
+      <c r="BK19" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sua dinh dang excel cho dep
</commit_message>
<xml_diff>
--- a/form_collectdata/form_collect/DataCollected/final_new.xlsx
+++ b/form_collectdata/form_collect/DataCollected/final_new.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK3"/>
+  <dimension ref="A1:BK11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -931,41 +931,6 @@
           <t>D20DTRB</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr">
         <is>
           <t>Mai Thị Nghĩa</t>
@@ -991,26 +956,791 @@
           <t>8.4</t>
         </is>
       </c>
-      <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="inlineStr"/>
-      <c r="AV3" t="inlineStr"/>
-      <c r="AW3" t="inlineStr"/>
-      <c r="AX3" t="inlineStr"/>
-      <c r="AY3" t="inlineStr"/>
-      <c r="AZ3" t="inlineStr"/>
-      <c r="BA3" t="inlineStr"/>
-      <c r="BB3" t="inlineStr"/>
-      <c r="BC3" t="inlineStr"/>
-      <c r="BD3" t="inlineStr"/>
-      <c r="BE3" t="inlineStr"/>
-      <c r="BF3" t="inlineStr"/>
-      <c r="BG3" t="inlineStr"/>
-      <c r="BH3" t="inlineStr"/>
-      <c r="BI3" t="inlineStr"/>
-      <c r="BJ3" t="inlineStr"/>
-      <c r="BK3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Xuân Tiến Vinh</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>B20DCDT227</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>D20XLTH</t>
+        </is>
+      </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>Nguyễn Quang Biên</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="BG4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BH4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="BI4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BJ4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BK4" t="inlineStr">
+        <is>
+          <t>6.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hướng Thành Nam</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B20DCDT143</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>D20XLTH</t>
+        </is>
+      </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>Nguyễn Quang Biên</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="BG5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BH5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BI5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="BJ5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="BK5" t="inlineStr">
+        <is>
+          <t>6.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Đinh Thế Vinh</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B20DCDT223</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>D20XLTH</t>
+        </is>
+      </c>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>Nguyễn Quang Biên</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="BG6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BH6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BI6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BJ6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BK6" t="inlineStr">
+        <is>
+          <t>5.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>La Thị Hồng Nhung</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>B20DCDT158</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>D20XLTH</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Phạm Hoàng Anh</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>7.6</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Chu Văn Bền</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>8.6</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Trần Thị Thục Linh</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>8.4</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>Nguyễn Văn Nghị</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>7.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Nguyễn Trung Tuấn</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>B20DCDT190</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>D20XLTH</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Phạm Hoàng Anh</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>6.4</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Chu Văn Bền</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>8.6</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Trần Thị Thục Linh</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>9.0</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>Nguyễn Văn Nghị</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>7.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Phạm Thế Anh</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>B20DCDT017</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>D20DTMT1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Đinh Quang Ngọc</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>6.4</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
+      <c r="AR9" t="inlineStr"/>
+      <c r="AS9" t="inlineStr"/>
+      <c r="AT9" t="inlineStr"/>
+      <c r="AU9" t="inlineStr"/>
+      <c r="AV9" t="inlineStr"/>
+      <c r="AW9" t="inlineStr"/>
+      <c r="AX9" t="inlineStr"/>
+      <c r="AY9" t="inlineStr"/>
+      <c r="AZ9" t="inlineStr"/>
+      <c r="BA9" t="inlineStr"/>
+      <c r="BB9" t="inlineStr"/>
+      <c r="BC9" t="inlineStr"/>
+      <c r="BD9" t="inlineStr"/>
+      <c r="BE9" t="inlineStr"/>
+      <c r="BF9" t="inlineStr"/>
+      <c r="BG9" t="inlineStr"/>
+      <c r="BH9" t="inlineStr"/>
+      <c r="BI9" t="inlineStr"/>
+      <c r="BJ9" t="inlineStr"/>
+      <c r="BK9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Nguyễn Tiến Duy</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>B20DCDT037</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>D20DTMT1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Đinh Quang Ngọc</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>7.4</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
+      <c r="AR10" t="inlineStr"/>
+      <c r="AS10" t="inlineStr"/>
+      <c r="AT10" t="inlineStr"/>
+      <c r="AU10" t="inlineStr"/>
+      <c r="AV10" t="inlineStr"/>
+      <c r="AW10" t="inlineStr"/>
+      <c r="AX10" t="inlineStr"/>
+      <c r="AY10" t="inlineStr"/>
+      <c r="AZ10" t="inlineStr"/>
+      <c r="BA10" t="inlineStr"/>
+      <c r="BB10" t="inlineStr"/>
+      <c r="BC10" t="inlineStr"/>
+      <c r="BD10" t="inlineStr"/>
+      <c r="BE10" t="inlineStr"/>
+      <c r="BF10" t="inlineStr"/>
+      <c r="BG10" t="inlineStr"/>
+      <c r="BH10" t="inlineStr"/>
+      <c r="BI10" t="inlineStr"/>
+      <c r="BJ10" t="inlineStr"/>
+      <c r="BK10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Lê Sỹ Sang</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>B20DCDT175</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>D20DTMT2</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Đinh Quang Ngọc</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>8.4</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
+      <c r="AR11" t="inlineStr"/>
+      <c r="AS11" t="inlineStr"/>
+      <c r="AT11" t="inlineStr"/>
+      <c r="AU11" t="inlineStr"/>
+      <c r="AV11" t="inlineStr"/>
+      <c r="AW11" t="inlineStr"/>
+      <c r="AX11" t="inlineStr"/>
+      <c r="AY11" t="inlineStr"/>
+      <c r="AZ11" t="inlineStr"/>
+      <c r="BA11" t="inlineStr"/>
+      <c r="BB11" t="inlineStr"/>
+      <c r="BC11" t="inlineStr"/>
+      <c r="BD11" t="inlineStr"/>
+      <c r="BE11" t="inlineStr"/>
+      <c r="BF11" t="inlineStr"/>
+      <c r="BG11" t="inlineStr"/>
+      <c r="BH11" t="inlineStr"/>
+      <c r="BI11" t="inlineStr"/>
+      <c r="BJ11" t="inlineStr"/>
+      <c r="BK11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>